<commit_message>
Tabelle Equipment um Feld "Anzahl" ergänzt
- ROOM Datenbank angepasst
- ROOM Migration hinzugefügt
- Datenbankvorlage angepasst
- ServerManager angepasst
</commit_message>
<xml_diff>
--- a/server/tools/Datenbank Template.xlsx
+++ b/server/tools/Datenbank Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tray" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="groupx" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">equipment!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">equipment!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">groupx!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">positionimage!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tray!$A$1:$G$13</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>id</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>Ein Rollwagen der anderen Gruppe, er besitzt kein Bild und keine Positionsmarkierungen</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -506,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,10 +695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,13 +712,14 @@
     <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="1"/>
+    <col min="10" max="10" width="8.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,16 +748,19 @@
         <v>9</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -776,16 +789,19 @@
         <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -814,17 +830,20 @@
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1">
+  <autoFilter ref="A1:L1">
     <sortState ref="A2:K402">
       <sortCondition ref="B1"/>
     </sortState>
@@ -911,7 +930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -982,7 +1001,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Server Managment API gegen Brute-Force abgesichert
Entsprechend #39 wurden Maßnahmen getroffen, um den Server gegen Brute-Force- oder Wörterbuchangriffe abzusichern.
</commit_message>
<xml_diff>
--- a/server/tools/Datenbank Template.xlsx
+++ b/server/tools/Datenbank Template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tray" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>id</t>
   </si>
@@ -171,12 +171,30 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>login_attempts</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>gesperrter_zugang</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,7 +533,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -529,19 +547,19 @@
       <selection activeCell="F11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -564,7 +582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -587,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -610,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
@@ -618,7 +636,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="4"/>
@@ -626,7 +644,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
@@ -634,7 +652,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
@@ -642,7 +660,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -650,13 +668,13 @@
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -664,7 +682,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -672,7 +690,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
@@ -680,7 +698,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -697,29 +715,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" style="2" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7109375" style="1"/>
+    <col min="13" max="13" width="13.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -760,7 +778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -801,7 +819,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -864,12 +882,12 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -903,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -928,18 +946,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,8 +973,14 @@
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -972,8 +996,14 @@
       <c r="E2" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -988,6 +1018,35 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1004,12 +1063,12 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1037,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>

</xml_diff>